<commit_message>
Testing variables structure. Fixing problem and variables files.
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_structure/input_data/input_data.xlsx
+++ b/tests/fixtures/test_structure/input_data/input_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\default\0_test_structure\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\fixtures\test_structure\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F7DD56-2624-41A4-B752-8532D31181DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1402A113-3EA3-4A9D-96B9-1354A99E71F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3870" yWindow="2770" windowWidth="23210" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31490" yWindow="1780" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V" sheetId="1" r:id="rId1"/>
@@ -450,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="K178" sqref="K178"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>